<commit_message>
Updated functionalities.Better code-3rd version
</commit_message>
<xml_diff>
--- a/PersonalTT/teacher_template.xlsx
+++ b/PersonalTT/teacher_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -286,28 +286,13 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -318,12 +303,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,6 +334,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -661,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I9" sqref="B4:I9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,85 +716,159 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>